<commit_message>
Adjustment QM region country definition
</commit_message>
<xml_diff>
--- a/data-input/country-codes/country-codes-core.xlsx
+++ b/data-input/country-codes/country-codes-core.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowaidamoshrif/Documents/GitHub/wid-world/data-input/country-codes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelestebanarias/Documents/GitHub/wid-world/data-input/country-codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA07A10B-2E4F-3F43-A279-B2E3D3A59199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4470F0AA-00ED-2040-BE1F-0734D1A10AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="500" windowWidth="30240" windowHeight="27200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5898" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5897" uniqueCount="1135">
   <si>
     <t>code</t>
   </si>
@@ -3813,8 +3813,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J737"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A491" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A734" sqref="A5:A734"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="84" workbookViewId="0">
+      <selection activeCell="G290" sqref="G290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12354,9 +12354,7 @@
       <c r="F290" t="s">
         <v>738</v>
       </c>
-      <c r="G290" s="2" t="s">
-        <v>918</v>
-      </c>
+      <c r="G290" s="2"/>
       <c r="H290" t="s">
         <v>943</v>
       </c>

</xml_diff>

<commit_message>
Correction to integration of pop data and new historical breakdowns
This commit:
1. Corrected the integration of the Federico Tena dataset.
2. Completed the estimation of the 997 aggregates.
3. Corrected the integration of the long-run estimates by substituting the historical estimates with the FT data.
4. Included extended age and gender breakdowns.
</commit_message>
<xml_diff>
--- a/data-input/country-codes/country-codes-core.xlsx
+++ b/data-input/country-codes/country-codes-core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelestebanarias/Documents/GitHub/wid-world/data-input/country-codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4470F0AA-00ED-2040-BE1F-0734D1A10AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BBDBAC-B5C3-DB4C-B0F8-F67CCC89F421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5897" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5893" uniqueCount="1135">
   <si>
     <t>code</t>
   </si>
@@ -3445,12 +3445,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3472,10 +3484,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3813,8 +3827,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J737"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="84" workbookViewId="0">
-      <selection activeCell="G290" sqref="G290"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="F341" sqref="F341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8803,9 +8817,7 @@
       <c r="E169" t="s">
         <v>962</v>
       </c>
-      <c r="F169" t="s">
-        <v>963</v>
-      </c>
+      <c r="F169" s="4"/>
       <c r="G169" t="s">
         <v>738</v>
       </c>
@@ -9019,9 +9031,7 @@
       <c r="E176" t="s">
         <v>962</v>
       </c>
-      <c r="F176" t="s">
-        <v>963</v>
-      </c>
+      <c r="F176" s="4"/>
       <c r="G176" t="s">
         <v>918</v>
       </c>
@@ -10655,9 +10665,7 @@
       <c r="E232" t="s">
         <v>962</v>
       </c>
-      <c r="F232" t="s">
-        <v>963</v>
-      </c>
+      <c r="F232" s="4"/>
       <c r="G232" t="s">
         <v>918</v>
       </c>
@@ -12348,7 +12356,7 @@
       <c r="D290" t="s">
         <v>943</v>
       </c>
-      <c r="E290" t="s">
+      <c r="E290" s="3" t="s">
         <v>951</v>
       </c>
       <c r="F290" t="s">
@@ -13885,9 +13893,7 @@
       <c r="E341" t="s">
         <v>1112</v>
       </c>
-      <c r="F341" t="s">
-        <v>963</v>
-      </c>
+      <c r="F341" s="4"/>
       <c r="G341" t="s">
         <v>919</v>
       </c>
@@ -15827,8 +15833,8 @@
       <c r="G407" s="2" t="s">
         <v>921</v>
       </c>
-      <c r="H407" t="s">
-        <v>1079</v>
+      <c r="H407" s="3" t="s">
+        <v>1072</v>
       </c>
       <c r="I407" s="1">
         <v>1</v>

</xml_diff>